<commit_message>
TopUp Loans 10 testcases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2481-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-AMT-VAR-INST-UPFRONT-Makerepayment2.xlsx
+++ b/Mifos Automation Excels/Client/2481-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-AMT-VAR-INST-UPFRONT-Makerepayment2.xlsx
@@ -20,7 +20,7 @@
     <sheet name="Acc_Repayment" sheetId="9" r:id="rId6"/>
     <sheet name="Acc_Disbursement1" sheetId="7" r:id="rId7"/>
     <sheet name="Acc_Repayment1" sheetId="6" r:id="rId8"/>
-    <sheet name="Acc_Upfront" sheetId="10" r:id="rId9"/>
+    <sheet name="Acc_Upfront" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -200,10 +200,10 @@
     <t>$ 877.73</t>
   </si>
   <si>
-    <t>L47</t>
-  </si>
-  <si>
-    <t>$ 543.84</t>
+    <t>L282</t>
+  </si>
+  <si>
+    <t>$ 543.84</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,22 +2264,12 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
@@ -2308,9 +2298,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>22</v>
@@ -2335,9 +2325,9 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>22</v>

</xml_diff>